<commit_message>
Circuit schematics update + LED power test sketch added
</commit_message>
<xml_diff>
--- a/DEMO_touch_MPR121_circuit/DEMO_touch_MPR121_circuit.xlsx
+++ b/DEMO_touch_MPR121_circuit/DEMO_touch_MPR121_circuit.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="v0" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="29">
   <si>
     <t>Reference</t>
   </si>
@@ -31,18 +32,9 @@
     <t xml:space="preserve"> Datasheet</t>
   </si>
   <si>
-    <t xml:space="preserve">J1 </t>
-  </si>
-  <si>
-    <t>Conn_01x10_Male</t>
-  </si>
-  <si>
     <t>~</t>
   </si>
   <si>
-    <t xml:space="preserve">JP1 </t>
-  </si>
-  <si>
     <t>HEADER-1X10</t>
   </si>
   <si>
@@ -98,6 +90,18 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>v0</t>
+  </si>
+  <si>
+    <t>JP1 JP2</t>
+  </si>
+  <si>
+    <t>lead wire</t>
+  </si>
+  <si>
+    <t>R2 R4 R5 R9</t>
   </si>
 </sst>
 </file>
@@ -173,8 +177,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Táblázat4" displayName="Táblázat4" ref="A3:E14" totalsRowShown="0">
-  <autoFilter ref="A3:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Táblázat4" displayName="Táblázat4" ref="A3:E13" totalsRowShown="0">
+  <autoFilter ref="A3:E13"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Reference"/>
+    <tableColumn id="2" name=" Quantity"/>
+    <tableColumn id="3" name=" Value"/>
+    <tableColumn id="4" name=" Footprint"/>
+    <tableColumn id="5" name=" Datasheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Táblázat42" displayName="Táblázat42" ref="A3:E12" totalsRowShown="0">
+  <autoFilter ref="A3:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Reference"/>
     <tableColumn id="2" name=" Quantity"/>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,11 +508,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -517,36 +538,36 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,161 +575,360 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1"/>
+    <hyperlink ref="E10" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="E13" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E11" r:id="rId2"/>
-    <hyperlink ref="E12" r:id="rId3"/>
-    <hyperlink ref="E13" r:id="rId4"/>
-    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E5" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E10" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="E12" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>